<commit_message>
English words added 3.3.0
</commit_message>
<xml_diff>
--- a/Excel/Top 1000 Words in Gilaki (English).xlsx
+++ b/Excel/Top 1000 Words in Gilaki (English).xlsx
@@ -5537,7 +5537,7 @@
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>Such A Big...</t>
+          <t>Such A Big…</t>
         </is>
       </c>
       <c r="D233" t="inlineStr">
@@ -16378,7 +16378,7 @@
       </c>
       <c r="B726" t="inlineStr">
         <is>
-          <t>أتؤ نيه کي...</t>
+          <t>أتؤ نيه کي…</t>
         </is>
       </c>
       <c r="C726" t="inlineStr">
@@ -16388,7 +16388,7 @@
       </c>
       <c r="D726" t="inlineStr">
         <is>
-          <t>It's not like that...</t>
+          <t>It's not like that…</t>
         </is>
       </c>
     </row>
@@ -18539,7 +18539,7 @@
       </c>
       <c r="C824" t="inlineStr">
         <is>
-          <t>It's Good That...</t>
+          <t>It's Good That…</t>
         </is>
       </c>
       <c r="D824" t="inlineStr">

</xml_diff>

<commit_message>
English words added 3.3.1
</commit_message>
<xml_diff>
--- a/Excel/Top 1000 Words in Gilaki (English).xlsx
+++ b/Excel/Top 1000 Words in Gilaki (English).xlsx
@@ -988,7 +988,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Nasser suddenly entered the room</t>
+          <t>Naser suddenly entered the room</t>
         </is>
       </c>
     </row>
@@ -1990,7 +1990,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>جه وس هوا سرده أمي دهنأ ألاو بيرۊن أيه</t>
+          <t>هوا سرده أمي دهنأ ألاو بيرۊن أيه</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2000,7 +2000,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>It's too cold that steam come from our mouth</t>
+          <t>It's cold that steam come from our mouth</t>
         </is>
       </c>
     </row>
@@ -3662,7 +3662,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>گيلان ٚ بجاران همه بي پا بؤستن دره</t>
+          <t>گيلان ٚ بجاران همه بي پا بؤستن دريد</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
@@ -5163,12 +5163,12 @@
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>In The Weeks</t>
+          <t>Far Away</t>
         </is>
       </c>
       <c r="D216" t="inlineStr">
         <is>
-          <t>Tiger on those weeks</t>
+          <t>Take these and throw them far away</t>
         </is>
       </c>
     </row>
@@ -5190,7 +5190,7 @@
       </c>
       <c r="D217" t="inlineStr">
         <is>
-          <t>he's a little boy, he craves</t>
+          <t>He's a little boy, he craves</t>
         </is>
       </c>
     </row>
@@ -6390,7 +6390,7 @@
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>أ زأى چقد ترکمه-يه؟</t>
+          <t>أ زأى چندر ترکمه-يه؟</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
@@ -12704,7 +12704,7 @@
       </c>
       <c r="B559" t="inlineStr">
         <is>
-          <t>جه وس هوا سرده سانچؤ زئن درم</t>
+          <t>هوا سرده سانچؤ زئن درم</t>
         </is>
       </c>
       <c r="C559" t="inlineStr">
@@ -12714,7 +12714,7 @@
       </c>
       <c r="D559" t="inlineStr">
         <is>
-          <t>It's too cold I'm getting pneumonia</t>
+          <t>It's cold I'm getting pneumonia</t>
         </is>
       </c>
     </row>
@@ -13914,7 +13914,7 @@
       </c>
       <c r="B614" t="inlineStr">
         <is>
-          <t>أيأ چقد گرمه، شه بزم</t>
+          <t>أيأ چندر گرمه، شه بزم</t>
         </is>
       </c>
       <c r="C614" t="inlineStr">

</xml_diff>

<commit_message>
English words added 3.3.2
</commit_message>
<xml_diff>
--- a/Excel/Top 1000 Words in Gilaki (English).xlsx
+++ b/Excel/Top 1000 Words in Gilaki (English).xlsx
@@ -2738,7 +2738,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>أن ٚ باقي بمانسته    ٰ چي بۊکۊنم؟</t>
+          <t>أن ٚ باقي بمانسته     ٰ چي بۊکۊنم؟</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -4564,7 +4564,7 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>أشان خأئيد همه    ٰ بۊکۊشيد</t>
+          <t>أشان خأئيد همه     ٰ بۊکۊشيد</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
@@ -5004,7 +5004,7 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>أمي مؤبل ٚ دسته    ٰ پت بزه</t>
+          <t>أمي مؤبل ٚ دسته     ٰ پت بزه</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
@@ -6962,7 +6962,7 @@
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>پارچهˈ همهˈ تۊرتۊره     ٰ کۊد</t>
+          <t>پارچهˈ همهˈ تۊرتۊره      ٰ کۊد</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
@@ -7226,7 +7226,7 @@
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>سجاد ؤ أکبر تۊکاپرهˈ ديبيد</t>
+          <t>فرزاد ؤ أحمد تۊکاپرهˈ ديبيد</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
@@ -7358,7 +7358,7 @@
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>تي وسيله    ٰن کابينت ٚ جؤر نهأ</t>
+          <t>تي وسيله     ٰن کابينت ٚ جؤر نهأ</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
@@ -7666,7 +7666,7 @@
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>خۊ وسيله    ٰنأ جيجاماما کۊدن دره</t>
+          <t>خۊ وسيله     ٰنأ جيجاماما کۊدن دره</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
@@ -8304,7 +8304,7 @@
       </c>
       <c r="B359" t="inlineStr">
         <is>
-          <t>پارچه     ٰ چارکۊنج واوين</t>
+          <t>پارچه      ٰ چارکۊنج واوين</t>
         </is>
       </c>
       <c r="C359" t="inlineStr">
@@ -8568,7 +8568,7 @@
       </c>
       <c r="B371" t="inlineStr">
         <is>
-          <t>چمچه    ٰ بيدئي؟</t>
+          <t>چمچه     ٰ بيدئي؟</t>
         </is>
       </c>
       <c r="C371" t="inlineStr">
@@ -11252,7 +11252,7 @@
       </c>
       <c r="B493" t="inlineStr">
         <is>
-          <t>ديرۊ شيمي کۊچه    ٰ دٚوارستم</t>
+          <t>ديرۊ شيمي کۊچه     ٰ دٚوارستم</t>
         </is>
       </c>
       <c r="C493" t="inlineStr">
@@ -12770,7 +12770,7 @@
       </c>
       <c r="B562" t="inlineStr">
         <is>
-          <t>تي وسيله    ٰنأ بنه ميز ٚ سر</t>
+          <t>تي وسيله     ٰنأ بنه ميز ٚ سر</t>
         </is>
       </c>
       <c r="C562" t="inlineStr">
@@ -13298,7 +13298,7 @@
       </c>
       <c r="B586" t="inlineStr">
         <is>
-          <t>سٚفره     ٰ بۊشؤستم</t>
+          <t>سٚفره      ٰ بۊشؤستم</t>
         </is>
       </c>
       <c r="C586" t="inlineStr">
@@ -15036,7 +15036,7 @@
       </c>
       <c r="B665" t="inlineStr">
         <is>
-          <t>سٚفره     ٰ فلگان</t>
+          <t>سٚفره      ٰ فلگان</t>
         </is>
       </c>
       <c r="C665" t="inlineStr">
@@ -16246,7 +16246,7 @@
       </c>
       <c r="B720" t="inlineStr">
         <is>
-          <t>بۊشۊ اۊ کلانه    ٰ بأور</t>
+          <t>بۊشۊ اۊ کلانه     ٰ بأور</t>
         </is>
       </c>
       <c r="C720" t="inlineStr">
@@ -16334,7 +16334,7 @@
       </c>
       <c r="B724" t="inlineStr">
         <is>
-          <t>بۊشۊ کله    ٰ وأگيران</t>
+          <t>بۊشۊ کله     ٰ وأگيران</t>
         </is>
       </c>
       <c r="C724" t="inlineStr">
@@ -16928,7 +16928,7 @@
       </c>
       <c r="B751" t="inlineStr">
         <is>
-          <t>جغله    ٰ ببر گاره دۊرۊن بۊخۊسان</t>
+          <t>جغله     ٰ ببر گاره دۊرۊن بۊخۊسان</t>
         </is>
       </c>
       <c r="C751" t="inlineStr">
@@ -17984,7 +17984,7 @@
       </c>
       <c r="B799" t="inlineStr">
         <is>
-          <t>اۊ لته    ٰ مرأ فأدن ميزأ پأکۊنم</t>
+          <t>اۊ لته     ٰ مرأ فأدن ميزأ پأکۊنم</t>
         </is>
       </c>
       <c r="C799" t="inlineStr">
@@ -18050,7 +18050,7 @@
       </c>
       <c r="B802" t="inlineStr">
         <is>
-          <t>لپه    ٰ تأود</t>
+          <t>لپه     ٰ تأود</t>
         </is>
       </c>
       <c r="C802" t="inlineStr">
@@ -18248,7 +18248,7 @@
       </c>
       <c r="B811" t="inlineStr">
         <is>
-          <t>مئوه    ٰنأ بۊشؤستي؟</t>
+          <t>مئوه     ٰنأ بۊشؤستي؟</t>
         </is>
       </c>
       <c r="C811" t="inlineStr">
@@ -19062,7 +19062,7 @@
       </c>
       <c r="B848" t="inlineStr">
         <is>
-          <t>أمين خۊ مچه    ٰ عمل بۊکۊده</t>
+          <t>أمين خۊ مچه     ٰ عمل بۊکۊده</t>
         </is>
       </c>
       <c r="C848" t="inlineStr">
@@ -20778,7 +20778,7 @@
       </c>
       <c r="B926" t="inlineStr">
         <is>
-          <t>ايپچه اۊشنتر همه    ٰ وارسي کۊديد</t>
+          <t>ايپچه اۊشنتر همه     ٰ وارسي کۊديد</t>
         </is>
       </c>
       <c r="C926" t="inlineStr">
@@ -20932,7 +20932,7 @@
       </c>
       <c r="B933" t="inlineStr">
         <is>
-          <t>اۊن چیسه تي دينأ وأسئن دري؟</t>
+          <t>اۊن چیسه تي ديمأ وأسئن دري؟</t>
         </is>
       </c>
       <c r="C933" t="inlineStr">
@@ -21174,7 +21174,7 @@
       </c>
       <c r="B944" t="inlineStr">
         <is>
-          <t>گاب خۊ مانده    ٰ واليشتن دره</t>
+          <t>گاب خۊ مانده     ٰ واليشتن دره</t>
         </is>
       </c>
       <c r="C944" t="inlineStr">
@@ -21614,7 +21614,7 @@
       </c>
       <c r="B964" t="inlineStr">
         <is>
-          <t>مي اينستا ولگأ دأري؟</t>
+          <t>مي اينستاگرام ولگأ دأري؟</t>
         </is>
       </c>
       <c r="C964" t="inlineStr">

</xml_diff>